<commit_message>
task 2 & task 1
</commit_message>
<xml_diff>
--- a/Task-1.xlsx
+++ b/Task-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA_ALL_TASK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C9D71D2-F8A8-48A7-9C22-93A8D41C6871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30444EE-502B-44C4-A72F-351ED16B7F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1766,6 +1766,42 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1778,12 +1814,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1805,45 +1835,57 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1853,47 +1895,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1907,29 +1931,41 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1956,42 +1992,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3605,21 +3605,21 @@
       <c r="R2" s="4"/>
     </row>
     <row r="3" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="204" t="s">
+      <c r="A3" s="195" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="205"/>
-      <c r="C3" s="205"/>
-      <c r="D3" s="205"/>
-      <c r="E3" s="206"/>
+      <c r="B3" s="196"/>
+      <c r="C3" s="196"/>
+      <c r="D3" s="196"/>
+      <c r="E3" s="197"/>
       <c r="F3" s="109"/>
-      <c r="G3" s="198" t="s">
+      <c r="G3" s="210" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="199"/>
-      <c r="I3" s="199"/>
-      <c r="J3" s="199"/>
-      <c r="K3" s="200"/>
+      <c r="H3" s="211"/>
+      <c r="I3" s="211"/>
+      <c r="J3" s="211"/>
+      <c r="K3" s="212"/>
       <c r="L3" s="95"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -3629,21 +3629,21 @@
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="207"/>
-      <c r="B4" s="208"/>
-      <c r="C4" s="208"/>
-      <c r="D4" s="208"/>
-      <c r="E4" s="209"/>
+      <c r="A4" s="198"/>
+      <c r="B4" s="199"/>
+      <c r="C4" s="199"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="200"/>
       <c r="F4" s="86"/>
-      <c r="G4" s="210" t="s">
+      <c r="G4" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="211"/>
-      <c r="I4" s="212"/>
-      <c r="J4" s="210" t="s">
+      <c r="H4" s="202"/>
+      <c r="I4" s="203"/>
+      <c r="J4" s="201" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="212"/>
+      <c r="K4" s="203"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -3656,15 +3656,15 @@
       <c r="B5" s="30"/>
       <c r="E5" s="30"/>
       <c r="F5" s="86"/>
-      <c r="G5" s="213" t="s">
+      <c r="G5" s="204" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="214"/>
-      <c r="I5" s="215"/>
-      <c r="J5" s="213" t="s">
+      <c r="H5" s="205"/>
+      <c r="I5" s="206"/>
+      <c r="J5" s="204" t="s">
         <v>86</v>
       </c>
-      <c r="K5" s="215"/>
+      <c r="K5" s="206"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -3682,15 +3682,15 @@
       <c r="D6" s="96"/>
       <c r="E6" s="111"/>
       <c r="F6" s="86"/>
-      <c r="G6" s="201" t="s">
+      <c r="G6" s="213" t="s">
         <v>87</v>
       </c>
-      <c r="H6" s="202"/>
-      <c r="I6" s="203"/>
-      <c r="J6" s="201" t="s">
+      <c r="H6" s="214"/>
+      <c r="I6" s="215"/>
+      <c r="J6" s="213" t="s">
         <v>88</v>
       </c>
-      <c r="K6" s="203"/>
+      <c r="K6" s="215"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -3708,15 +3708,15 @@
       <c r="D7" s="110"/>
       <c r="E7" s="111"/>
       <c r="F7" s="86"/>
-      <c r="G7" s="201" t="s">
+      <c r="G7" s="213" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="202"/>
-      <c r="I7" s="203"/>
-      <c r="J7" s="201" t="s">
+      <c r="H7" s="214"/>
+      <c r="I7" s="215"/>
+      <c r="J7" s="213" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="203"/>
+      <c r="K7" s="215"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -3732,15 +3732,15 @@
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="86"/>
-      <c r="G8" s="201" t="s">
+      <c r="G8" s="213" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="202"/>
-      <c r="I8" s="203"/>
-      <c r="J8" s="201" t="s">
+      <c r="H8" s="214"/>
+      <c r="I8" s="215"/>
+      <c r="J8" s="213" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="203"/>
+      <c r="K8" s="215"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -3751,15 +3751,15 @@
     </row>
     <row r="9" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F9" s="86"/>
-      <c r="G9" s="195" t="s">
+      <c r="G9" s="207" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="196"/>
-      <c r="I9" s="197"/>
-      <c r="J9" s="195" t="s">
+      <c r="H9" s="208"/>
+      <c r="I9" s="209"/>
+      <c r="J9" s="207" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="197"/>
+      <c r="K9" s="209"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -4772,11 +4772,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A3:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="G3:K3"/>
@@ -4786,6 +4781,11 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A3:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4797,7 +4797,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4820,7 +4820,10 @@
       <c r="A2" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="59"/>
+      <c r="B2" s="59" cm="1">
+        <f t="array" ref="B2">SUMPRODUCT(--(LEN(A4:F10)=2))</f>
+        <v>24</v>
+      </c>
       <c r="C2" s="59"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
@@ -5141,8 +5144,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P440"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9299,8 +9302,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9659,16 +9662,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="140" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="155"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="142"/>
       <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9682,7 +9685,7 @@
       <c r="A3" s="116" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="156" t="s">
+      <c r="B3" s="143" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="144"/>
@@ -9696,57 +9699,57 @@
       <c r="A4" s="115">
         <v>1</v>
       </c>
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="146" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="158"/>
-      <c r="D4" s="158"/>
-      <c r="E4" s="158"/>
-      <c r="F4" s="158"/>
-      <c r="G4" s="158"/>
-      <c r="H4" s="159"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="147"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="148"/>
     </row>
     <row r="5" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="113">
         <v>2</v>
       </c>
-      <c r="B5" s="157" t="s">
+      <c r="B5" s="146" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="158"/>
-      <c r="D5" s="158"/>
-      <c r="E5" s="158"/>
-      <c r="F5" s="158"/>
-      <c r="G5" s="158"/>
-      <c r="H5" s="159"/>
+      <c r="C5" s="147"/>
+      <c r="D5" s="147"/>
+      <c r="E5" s="147"/>
+      <c r="F5" s="147"/>
+      <c r="G5" s="147"/>
+      <c r="H5" s="148"/>
       <c r="I5" s="25"/>
     </row>
     <row r="6" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="114">
         <v>3</v>
       </c>
-      <c r="B6" s="160" t="s">
+      <c r="B6" s="149" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="161"/>
-      <c r="D6" s="161"/>
-      <c r="E6" s="161"/>
-      <c r="F6" s="161"/>
-      <c r="G6" s="161"/>
-      <c r="H6" s="162"/>
+      <c r="C6" s="150"/>
+      <c r="D6" s="150"/>
+      <c r="E6" s="150"/>
+      <c r="F6" s="150"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="151"/>
       <c r="I6" s="25"/>
     </row>
     <row r="7" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:9" ht="18.600000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="140" t="s">
+      <c r="A8" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="143" t="s">
+      <c r="B8" s="155" t="s">
         <v>119</v>
       </c>
       <c r="C8" s="144"/>
       <c r="D8" s="144"/>
-      <c r="E8" s="143" t="s">
+      <c r="E8" s="155" t="s">
         <v>120</v>
       </c>
       <c r="F8" s="144"/>
@@ -9754,49 +9757,49 @@
       <c r="H8" s="145"/>
     </row>
     <row r="9" spans="1:9" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="141"/>
-      <c r="B9" s="149" t="s">
+      <c r="A9" s="153"/>
+      <c r="B9" s="159" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="150"/>
-      <c r="D9" s="151"/>
-      <c r="E9" s="146">
+      <c r="C9" s="160"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="156">
         <f xml:space="preserve"> (  LEN(B4)    -LEN(SUBSTITUTE(B4,B9,"")) )  /  (LEN(B9))</f>
         <v>3</v>
       </c>
-      <c r="F9" s="147"/>
-      <c r="G9" s="147"/>
-      <c r="H9" s="148"/>
+      <c r="F9" s="157"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="158"/>
     </row>
     <row r="10" spans="1:9" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="141"/>
-      <c r="B10" s="152" t="s">
+      <c r="A10" s="153"/>
+      <c r="B10" s="162" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="152"/>
-      <c r="D10" s="152"/>
-      <c r="E10" s="146">
+      <c r="C10" s="162"/>
+      <c r="D10" s="162"/>
+      <c r="E10" s="156">
         <f t="shared" ref="E10:E11" si="0" xml:space="preserve"> (  LEN(B5)    -LEN(SUBSTITUTE(B5,B10,"")) )  /  (LEN(B10))</f>
         <v>2</v>
       </c>
-      <c r="F10" s="147"/>
-      <c r="G10" s="147"/>
-      <c r="H10" s="148"/>
+      <c r="F10" s="157"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="158"/>
     </row>
     <row r="11" spans="1:9" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="142"/>
-      <c r="B11" s="152" t="s">
+      <c r="A11" s="154"/>
+      <c r="B11" s="162" t="s">
         <v>126</v>
       </c>
-      <c r="C11" s="152"/>
-      <c r="D11" s="152"/>
-      <c r="E11" s="146">
+      <c r="C11" s="162"/>
+      <c r="D11" s="162"/>
+      <c r="E11" s="156">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F11" s="147"/>
-      <c r="G11" s="147"/>
-      <c r="H11" s="148"/>
+      <c r="F11" s="157"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="158"/>
       <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -9806,11 +9809,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="E9:H9"/>
@@ -9820,6 +9818,11 @@
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9842,30 +9845,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="166" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="171"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="168"/>
     </row>
     <row r="2" spans="1:13" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="172"/>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="174"/>
+      <c r="A2" s="169"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="171"/>
     </row>
     <row r="3" spans="1:13" s="17" customFormat="1" ht="21.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="123"/>
@@ -9881,18 +9884,18 @@
       <c r="K3" s="118"/>
     </row>
     <row r="4" spans="1:13" s="17" customFormat="1" ht="21.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="175" t="s">
+      <c r="A4" s="172" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="175"/>
-      <c r="C4" s="175"/>
-      <c r="D4" s="175"/>
-      <c r="E4" s="175"/>
-      <c r="F4" s="175"/>
-      <c r="G4" s="175"/>
-      <c r="H4" s="175"/>
-      <c r="I4" s="175"/>
-      <c r="J4" s="176"/>
+      <c r="B4" s="172"/>
+      <c r="C4" s="172"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="172"/>
+      <c r="F4" s="172"/>
+      <c r="G4" s="172"/>
+      <c r="H4" s="172"/>
+      <c r="I4" s="172"/>
+      <c r="J4" s="173"/>
       <c r="K4" s="121"/>
       <c r="M4"/>
     </row>
@@ -9900,16 +9903,16 @@
       <c r="A5" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="155" t="s">
         <v>119</v>
       </c>
       <c r="C5" s="144"/>
       <c r="D5" s="145"/>
-      <c r="E5" s="143" t="s">
+      <c r="E5" s="155" t="s">
         <v>138</v>
       </c>
       <c r="F5" s="145"/>
-      <c r="G5" s="143" t="s">
+      <c r="G5" s="155" t="s">
         <v>137</v>
       </c>
       <c r="H5" s="144"/>
@@ -9920,132 +9923,132 @@
       <c r="A6" s="120">
         <v>1</v>
       </c>
-      <c r="B6" s="180" t="s">
+      <c r="B6" s="174" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="182"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="180" t="s">
+      <c r="C6" s="178"/>
+      <c r="D6" s="175"/>
+      <c r="E6" s="174" t="s">
         <v>132</v>
       </c>
-      <c r="F6" s="181"/>
-      <c r="G6" s="177" t="str" cm="1">
+      <c r="F6" s="175"/>
+      <c r="G6" s="163" t="str" cm="1">
         <f t="array" ref="G6" xml:space="preserve"> PROPER(   _xlfn.SWITCH(E6, "F", "Mrs.",  "Mr." )&amp; " " &amp;RIGHT(B6,LEN(B6)-(SEARCH(",",B6)))&amp;  " " &amp;LEFT(B6,SEARCH(",",B6)-1) )</f>
         <v>Mrs. Bharti Gupta</v>
       </c>
-      <c r="H6" s="178"/>
-      <c r="I6" s="178"/>
-      <c r="J6" s="179"/>
+      <c r="H6" s="164"/>
+      <c r="I6" s="164"/>
+      <c r="J6" s="165"/>
       <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="122">
         <v>2</v>
       </c>
-      <c r="B7" s="163" t="s">
+      <c r="B7" s="176" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="164"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="163" t="s">
+      <c r="C7" s="179"/>
+      <c r="D7" s="177"/>
+      <c r="E7" s="176" t="s">
         <v>129</v>
       </c>
-      <c r="F7" s="165"/>
-      <c r="G7" s="177" t="str" cm="1">
+      <c r="F7" s="177"/>
+      <c r="G7" s="163" t="str" cm="1">
         <f t="array" ref="G7" xml:space="preserve"> PROPER(   _xlfn.SWITCH(E7, "F", "Mrs.",  "Mr." )&amp; " " &amp;RIGHT(B7,LEN(B7)-(SEARCH(",",B7)))&amp;  " " &amp;LEFT(B7,SEARCH(",",B7)-1) )</f>
         <v>Mr. Chandan Negi</v>
       </c>
-      <c r="H7" s="178"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="179"/>
+      <c r="H7" s="164"/>
+      <c r="I7" s="164"/>
+      <c r="J7" s="165"/>
       <c r="K7" s="25"/>
     </row>
     <row r="8" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="119">
         <v>3</v>
       </c>
-      <c r="B8" s="163" t="s">
+      <c r="B8" s="176" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="164"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="163" t="s">
+      <c r="C8" s="179"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="176" t="s">
         <v>132</v>
       </c>
-      <c r="F8" s="165"/>
-      <c r="G8" s="177" t="str" cm="1">
+      <c r="F8" s="177"/>
+      <c r="G8" s="163" t="str" cm="1">
         <f t="array" ref="G8" xml:space="preserve"> PROPER(   _xlfn.SWITCH(E8, "F", "Mrs.",  "Mr." )&amp; " " &amp;RIGHT(B8,LEN(B8)-(SEARCH(",",B8)))&amp;  " " &amp;LEFT(B8,SEARCH(",",B8)-1) )</f>
         <v>Mrs. Neha Malhotra</v>
       </c>
-      <c r="H8" s="178"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="179"/>
+      <c r="H8" s="164"/>
+      <c r="I8" s="164"/>
+      <c r="J8" s="165"/>
       <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="119">
         <v>4</v>
       </c>
-      <c r="B9" s="163" t="s">
+      <c r="B9" s="176" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="164"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="163" t="s">
+      <c r="C9" s="179"/>
+      <c r="D9" s="177"/>
+      <c r="E9" s="176" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="165"/>
-      <c r="G9" s="177" t="str" cm="1">
+      <c r="F9" s="177"/>
+      <c r="G9" s="163" t="str" cm="1">
         <f t="array" ref="G9" xml:space="preserve"> PROPER(   _xlfn.SWITCH(E9, "F", "Mrs.",  "Mr." )&amp; " " &amp;RIGHT(B9,LEN(B9)-(SEARCH(",",B9)))&amp;  " " &amp;LEFT(B9,SEARCH(",",B9)-1) )</f>
         <v>Mrs. Daljeet Kaur</v>
       </c>
-      <c r="H9" s="178"/>
-      <c r="I9" s="178"/>
-      <c r="J9" s="179"/>
+      <c r="H9" s="164"/>
+      <c r="I9" s="164"/>
+      <c r="J9" s="165"/>
       <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="119">
         <v>5</v>
       </c>
-      <c r="B10" s="163" t="s">
+      <c r="B10" s="176" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="164"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="163" t="s">
+      <c r="C10" s="179"/>
+      <c r="D10" s="177"/>
+      <c r="E10" s="176" t="s">
         <v>129</v>
       </c>
-      <c r="F10" s="165"/>
-      <c r="G10" s="177" t="str" cm="1">
+      <c r="F10" s="177"/>
+      <c r="G10" s="163" t="str" cm="1">
         <f t="array" ref="G10" xml:space="preserve"> PROPER(   _xlfn.SWITCH(E10, "F", "Mrs.",  "Mr." )&amp; " " &amp;RIGHT(B10,LEN(B10)-(SEARCH(",",B10)))&amp;  " " &amp;LEFT(B10,SEARCH(",",B10)-1) )</f>
         <v>Mr. Virit Shukla</v>
       </c>
-      <c r="H10" s="178"/>
-      <c r="I10" s="178"/>
-      <c r="J10" s="179"/>
+      <c r="H10" s="164"/>
+      <c r="I10" s="164"/>
+      <c r="J10" s="165"/>
       <c r="K10" s="25"/>
     </row>
     <row r="11" spans="1:13" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="119">
         <v>6</v>
       </c>
-      <c r="B11" s="166" t="s">
+      <c r="B11" s="180" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="168"/>
-      <c r="D11" s="167"/>
-      <c r="E11" s="166" t="s">
+      <c r="C11" s="182"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="180" t="s">
         <v>129</v>
       </c>
-      <c r="F11" s="167"/>
-      <c r="G11" s="177" t="str" cm="1">
+      <c r="F11" s="181"/>
+      <c r="G11" s="163" t="str" cm="1">
         <f t="array" ref="G11" xml:space="preserve"> PROPER(   _xlfn.SWITCH(E11, "F", "Mrs.",  "Mr." )&amp; " " &amp;RIGHT(B11,LEN(B11)-(SEARCH(",",B11)))&amp;  " " &amp;LEFT(B11,SEARCH(",",B11)-1) )</f>
         <v>Mr. Priyank Agarwal</v>
       </c>
-      <c r="H11" s="178"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="179"/>
+      <c r="H11" s="164"/>
+      <c r="I11" s="164"/>
+      <c r="J11" s="165"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
@@ -10054,6 +10057,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="G10:J10"/>
@@ -10070,13 +10080,6 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10087,124 +10090,124 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="G5" sqref="G5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="183" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="184"/>
+      <c r="F1" s="184"/>
+      <c r="G1" s="184"/>
+      <c r="H1" s="184"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="183" t="s">
+      <c r="A3" s="191" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="184"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="184"/>
-      <c r="G3" s="184"/>
-      <c r="H3" s="184"/>
+      <c r="B3" s="192"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
       <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="126" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="189" t="s">
+      <c r="B4" s="185" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
-      <c r="F4" s="191"/>
-      <c r="G4" s="185" t="s">
+      <c r="C4" s="186"/>
+      <c r="D4" s="186"/>
+      <c r="E4" s="186"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="193" t="s">
         <v>145</v>
       </c>
-      <c r="H4" s="186"/>
+      <c r="H4" s="194"/>
       <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="127">
         <v>1</v>
       </c>
-      <c r="B5" s="192" t="s">
+      <c r="B5" s="188" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="193"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="146" t="str">
+      <c r="C5" s="189"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="189"/>
+      <c r="F5" s="190"/>
+      <c r="G5" s="156" t="str">
         <f>RIGHT(B5,LEN(B5)-(SEARCH("check",B5)+7))</f>
         <v>12345</v>
       </c>
-      <c r="H5" s="148"/>
+      <c r="H5" s="158"/>
       <c r="I5" s="25"/>
     </row>
     <row r="6" spans="1:9" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="125">
         <v>2</v>
       </c>
-      <c r="B6" s="157" t="s">
+      <c r="B6" s="146" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158"/>
-      <c r="E6" s="158"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="146" t="str">
+      <c r="C6" s="147"/>
+      <c r="D6" s="147"/>
+      <c r="E6" s="147"/>
+      <c r="F6" s="148"/>
+      <c r="G6" s="156" t="str">
         <f t="shared" ref="G6:G8" si="0">RIGHT(B6,LEN(B6)-(SEARCH("check",B6)+7))</f>
         <v>123456</v>
       </c>
-      <c r="H6" s="148"/>
+      <c r="H6" s="158"/>
       <c r="I6" s="25"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="125">
         <v>3</v>
       </c>
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="146" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="159"/>
-      <c r="G7" s="146" t="str">
+      <c r="C7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="148"/>
+      <c r="G7" s="156" t="str">
         <f t="shared" si="0"/>
         <v>000789</v>
       </c>
-      <c r="H7" s="148"/>
+      <c r="H7" s="158"/>
       <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="125">
         <v>4</v>
       </c>
-      <c r="B8" s="160" t="s">
+      <c r="B8" s="149" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="161"/>
-      <c r="D8" s="161"/>
-      <c r="E8" s="161"/>
-      <c r="F8" s="162"/>
-      <c r="G8" s="146" t="str">
+      <c r="C8" s="150"/>
+      <c r="D8" s="150"/>
+      <c r="E8" s="150"/>
+      <c r="F8" s="151"/>
+      <c r="G8" s="156" t="str">
         <f t="shared" si="0"/>
         <v>123456</v>
       </c>
-      <c r="H8" s="148"/>
+      <c r="H8" s="158"/>
       <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -10212,11 +10215,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="G4:H4"/>
@@ -10224,6 +10222,11 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>